<commit_message>
Update Assignment with PR reference
</commit_message>
<xml_diff>
--- a/AssignmentReport.xlsx
+++ b/AssignmentReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhavala.Keerthi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priya.Ranpura\MRIInterns2026A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FBE34F-599C-4AD6-8D4B-12A6367172CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFC9D6C-F4D6-42B6-B09A-F8344D0645FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>PR Refs. [Comma seperated if there are multiple]</t>
+  </si>
+  <si>
+    <t>Priya.ranpura by PriyaRanpura · Pull Request #7 · dhavalkeerthi/MRIInterns2026A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +146,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,16 +172,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,16 +466,16 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -469,132 +483,138 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B16" r:id="rId1" display="https://github.com/dhavalkeerthi/MRIInterns2026A/pull/7" xr:uid="{154E38D6-63FF-40AA-9C4D-F24E2E2ED517}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add PR Refence link: uthpal.suvarna
</commit_message>
<xml_diff>
--- a/AssignmentReport.xlsx
+++ b/AssignmentReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhavala.Keerthi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uthpal.Suvarna\Projects\MRIInterns2026A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FBE34F-599C-4AD6-8D4B-12A6367172CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5B442F-C233-4AB3-80CA-54AA8090534D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>PR Refs. [Comma seperated if there are multiple]</t>
+  </si>
+  <si>
+    <t>Added Uthpal.Suvarna.txt by UthpalSuvarna · Pull Request #3 · dhavalkeerthi/MRIInterns2026A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +146,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,16 +172,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,16 +466,16 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -469,132 +483,138 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1" display="https://github.com/dhavalkeerthi/MRIInterns2026A/pull/3" xr:uid="{30727882-432A-4733-AF8B-2AE43DED8641}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Pull Request Reference
</commit_message>
<xml_diff>
--- a/AssignmentReport.xlsx
+++ b/AssignmentReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhavala.Keerthi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uthpal.Suvarna\Projects\MRIInterns2026A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FBE34F-599C-4AD6-8D4B-12A6367172CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51ABF81-EB22-419A-A4DB-83F41EED5808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>PR Refs. [Comma seperated if there are multiple]</t>
+  </si>
+  <si>
+    <t>Added Uthpal.Suvarna.txt by UthpalSuvarna · Pull Request #3 · dhavalkeerthi/MRIInterns2026A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +146,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,16 +172,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,16 +466,16 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -469,132 +483,138 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1" display="https://github.com/dhavalkeerthi/MRIInterns2026A/pull/3" xr:uid="{115A803C-71A8-406B-BBB9-1D405A411A97}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Pull Request Refernece - Navya.Yogish
</commit_message>
<xml_diff>
--- a/AssignmentReport.xlsx
+++ b/AssignmentReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhavala.Keerthi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navya.Yogish\MRIInterns2026A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FBE34F-599C-4AD6-8D4B-12A6367172CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111D672B-21DB-4654-AB16-9B17719B38DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>PR Refs. [Comma seperated if there are multiple]</t>
+  </si>
+  <si>
+    <t>demo by NavyaKKulal · Pull Request #11 · dhavalkeerthi/MRIInterns2026A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +146,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,16 +172,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,16 +466,16 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -469,132 +483,138 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1" display="https://github.com/dhavalkeerthi/MRIInterns2026A/pull/11" xr:uid="{4B98450E-9A0E-42C3-B0EE-9C78FD514079}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AssignmentReport updated by Harshith.Rai
</commit_message>
<xml_diff>
--- a/AssignmentReport.xlsx
+++ b/AssignmentReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhavala.Keerthi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshith.Rai\Desktop\github\MRIInterns2026A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FBE34F-599C-4AD6-8D4B-12A6367172CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2D19B8-7AB1-4422-9C06-5BEE2BB78D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>PR Refs. [Comma seperated if there are multiple]</t>
+  </si>
+  <si>
+    <t>Pull request #10 https://github.com/dhavalkeerthi/MRIInterns2026A/pull/10</t>
   </si>
 </sst>
 </file>
@@ -451,17 +454,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -469,127 +472,130 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Add pull request reference-Annika.Prasanna
</commit_message>
<xml_diff>
--- a/AssignmentReport.xlsx
+++ b/AssignmentReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhavala.Keerthi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annika.Prasanna\MRIInterns2026A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FBE34F-599C-4AD6-8D4B-12A6367172CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C86688-9B8E-4163-820A-FEB7159EF37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>PR Refs. [Comma seperated if there are multiple]</t>
+  </si>
+  <si>
+    <t>https://github.com/dhavalkeerthi/MRIInterns2026A/pull/27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +146,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,16 +172,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,16 +466,16 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -469,132 +483,138 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{C83456F5-1F67-49AA-9BE9-EA3892FB9D0E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added pull request reference
</commit_message>
<xml_diff>
--- a/AssignmentReport.xlsx
+++ b/AssignmentReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uthpal.Suvarna\Projects\MRIInterns2026A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\MRIInterns2026A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5B442F-C233-4AB3-80CA-54AA8090534D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6BF062-439B-4404-8DB6-30440096CF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Added Uthpal.Suvarna.txt by UthpalSuvarna · Pull Request #3 · dhavalkeerthi/MRIInterns2026A</t>
+  </si>
+  <si>
+    <t>https://github.com/dhavalkeerthi/MRIInterns2026A/pull/5</t>
   </si>
 </sst>
 </file>
@@ -465,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,6 +565,9 @@
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -614,6 +620,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B20" r:id="rId1" display="https://github.com/dhavalkeerthi/MRIInterns2026A/pull/3" xr:uid="{30727882-432A-4733-AF8B-2AE43DED8641}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{4FCDADA6-7661-4E68-AFDE-52F43AA2A906}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>